<commit_message>
Latest update to all Excel results files
Added results of using proc.time() to measure training and testing time on each experiment.
Added Notes sheet to results-store-7.xlsx to describe the contents of the fields
</commit_message>
<xml_diff>
--- a/results-store-1.xlsx
+++ b/results-store-1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://universityofsussex-my.sharepoint.com/personal/eh555_sussex_ac_uk/Documents/Documents/2-Proposal/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="90" documentId="8_{372AA814-B1E8-4BDB-8C12-AF40424DF215}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E777D87F-C852-4F62-9253-BE8B270BC8C9}"/>
+  <xr:revisionPtr revIDLastSave="129" documentId="8_{372AA814-B1E8-4BDB-8C12-AF40424DF215}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9F1F1D83-0C61-4719-86BF-E33CEF4E0F41}"/>
   <bookViews>
-    <workbookView xWindow="-28620" yWindow="60" windowWidth="28650" windowHeight="14550" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28605" yWindow="165" windowWidth="28650" windowHeight="14550" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="train_per_model" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="test_per_K" sheetId="6" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -57,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1288" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1385" uniqueCount="132">
   <si>
     <t>layers</t>
   </si>
@@ -473,6 +474,12 @@
   <si>
     <t>Tested with K range of 0.25 to 4</t>
   </si>
+  <si>
+    <t>Run with Laptop, using proc.time()</t>
+  </si>
+  <si>
+    <t>Again with K range of 0.25 to 4</t>
+  </si>
 </sst>
 </file>
 
@@ -545,7 +552,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
@@ -553,7 +560,6 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -883,10 +889,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P1233"/>
+  <dimension ref="A1:P1225"/>
   <sheetViews>
-    <sheetView topLeftCell="A103" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="J123" sqref="J123"/>
+    <sheetView topLeftCell="A100" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A126" sqref="A126:P127"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2048,10 +2054,7 @@
       </c>
       <c r="J37" s="3"/>
       <c r="K37" s="3"/>
-      <c r="L37" s="2">
-        <f>+L35-L32</f>
-        <v>-2.2477944838783599E-7</v>
-      </c>
+      <c r="L37" s="2"/>
       <c r="M37" s="2"/>
       <c r="N37" s="2"/>
       <c r="O37" s="2"/>
@@ -2059,10 +2062,7 @@
     <row r="38" spans="1:15" x14ac:dyDescent="0.25">
       <c r="J38" s="3"/>
       <c r="K38" s="3"/>
-      <c r="L38" s="2">
-        <f>+L37/L32</f>
-        <v>-0.31639643794137179</v>
-      </c>
+      <c r="L38" s="2"/>
       <c r="M38" s="2"/>
       <c r="N38" s="2"/>
       <c r="O38" s="2"/>
@@ -4138,7 +4138,7 @@
       <c r="O107" s="2"/>
     </row>
     <row r="108" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A108" s="7" t="s">
+      <c r="A108" t="s">
         <v>0</v>
       </c>
       <c r="B108" t="s">
@@ -4185,7 +4185,7 @@
       </c>
     </row>
     <row r="109" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A109" s="7">
+      <c r="A109">
         <v>2</v>
       </c>
       <c r="B109">
@@ -4643,31 +4643,31 @@
         <v>0.3</v>
       </c>
       <c r="G123" s="4">
-        <v>7.9799999999999999E-4</v>
+        <v>7.9778947561652297E-4</v>
       </c>
       <c r="H123" s="4">
-        <v>3.3372666000000002E-2</v>
+        <v>3.3372666097867897E-2</v>
       </c>
       <c r="I123" s="6">
-        <v>0.99999627000000002</v>
+        <v>0.99999627004511005</v>
       </c>
       <c r="J123" s="3">
-        <v>379.87327169999998</v>
+        <v>854.02</v>
       </c>
       <c r="K123" s="3">
-        <v>14.71734142</v>
+        <v>22.1924999999999</v>
       </c>
       <c r="L123" s="2">
-        <v>8.2399999999999997E-8</v>
+        <v>8.2375072096851896E-8</v>
       </c>
       <c r="M123" s="2">
-        <v>7.0799999999999999E-8</v>
+        <v>7.0835011236042895E-8</v>
       </c>
       <c r="N123" s="2">
-        <v>7.1400000000000004E-8</v>
+        <v>7.1376671500348307E-8</v>
       </c>
       <c r="O123" s="2">
-        <v>6.7599999999999997E-8</v>
+        <v>6.7627642238887299E-8</v>
       </c>
       <c r="P123" t="s">
         <v>118</v>
@@ -4682,6 +4682,9 @@
       <c r="O124" s="2"/>
     </row>
     <row r="125" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A125" s="1" t="s">
+        <v>130</v>
+      </c>
       <c r="J125" s="3"/>
       <c r="K125" s="3"/>
       <c r="L125" s="2"/>
@@ -4690,20 +4693,104 @@
       <c r="O125" s="2"/>
     </row>
     <row r="126" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="J126" s="3"/>
-      <c r="K126" s="3"/>
-      <c r="L126" s="2"/>
-      <c r="M126" s="2"/>
-      <c r="N126" s="2"/>
-      <c r="O126" s="2"/>
+      <c r="A126" t="s">
+        <v>0</v>
+      </c>
+      <c r="B126" t="s">
+        <v>1</v>
+      </c>
+      <c r="C126" t="s">
+        <v>28</v>
+      </c>
+      <c r="D126" t="s">
+        <v>29</v>
+      </c>
+      <c r="E126" t="s">
+        <v>2</v>
+      </c>
+      <c r="F126" t="s">
+        <v>3</v>
+      </c>
+      <c r="G126" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="H126" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="I126" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="J126" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="K126" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="L126" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="M126" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="N126" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="O126" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="P126" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="127" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="J127" s="3"/>
-      <c r="K127" s="3"/>
-      <c r="L127" s="2"/>
-      <c r="M127" s="2"/>
-      <c r="N127" s="2"/>
-      <c r="O127" s="2"/>
+      <c r="A127">
+        <v>2</v>
+      </c>
+      <c r="B127">
+        <v>1</v>
+      </c>
+      <c r="C127">
+        <v>4</v>
+      </c>
+      <c r="D127">
+        <v>1</v>
+      </c>
+      <c r="E127">
+        <v>710880</v>
+      </c>
+      <c r="F127">
+        <v>0.3</v>
+      </c>
+      <c r="G127" s="4">
+        <v>7.9778947561652297E-4</v>
+      </c>
+      <c r="H127" s="4">
+        <v>3.3372666097867897E-2</v>
+      </c>
+      <c r="I127" s="6">
+        <v>0.99999627004511005</v>
+      </c>
+      <c r="J127" s="3">
+        <v>401.93</v>
+      </c>
+      <c r="K127" s="3">
+        <v>11.805</v>
+      </c>
+      <c r="L127" s="2">
+        <v>8.2375072096851896E-8</v>
+      </c>
+      <c r="M127" s="2">
+        <v>7.0835011236042895E-8</v>
+      </c>
+      <c r="N127" s="2">
+        <v>7.1376671500348307E-8</v>
+      </c>
+      <c r="O127" s="2">
+        <v>6.7627642238887299E-8</v>
+      </c>
+      <c r="P127" t="s">
+        <v>118</v>
+      </c>
     </row>
     <row r="128" spans="1:16" x14ac:dyDescent="0.25">
       <c r="J128" s="3"/>
@@ -13488,70 +13575,6 @@
       <c r="M1225" s="2"/>
       <c r="N1225" s="2"/>
       <c r="O1225" s="2"/>
-    </row>
-    <row r="1226" spans="10:15" x14ac:dyDescent="0.25">
-      <c r="J1226" s="3"/>
-      <c r="K1226" s="3"/>
-      <c r="L1226" s="2"/>
-      <c r="M1226" s="2"/>
-      <c r="N1226" s="2"/>
-      <c r="O1226" s="2"/>
-    </row>
-    <row r="1227" spans="10:15" x14ac:dyDescent="0.25">
-      <c r="J1227" s="3"/>
-      <c r="K1227" s="3"/>
-      <c r="L1227" s="2"/>
-      <c r="M1227" s="2"/>
-      <c r="N1227" s="2"/>
-      <c r="O1227" s="2"/>
-    </row>
-    <row r="1228" spans="10:15" x14ac:dyDescent="0.25">
-      <c r="J1228" s="3"/>
-      <c r="K1228" s="3"/>
-      <c r="L1228" s="2"/>
-      <c r="M1228" s="2"/>
-      <c r="N1228" s="2"/>
-      <c r="O1228" s="2"/>
-    </row>
-    <row r="1229" spans="10:15" x14ac:dyDescent="0.25">
-      <c r="J1229" s="3"/>
-      <c r="K1229" s="3"/>
-      <c r="L1229" s="2"/>
-      <c r="M1229" s="2"/>
-      <c r="N1229" s="2"/>
-      <c r="O1229" s="2"/>
-    </row>
-    <row r="1230" spans="10:15" x14ac:dyDescent="0.25">
-      <c r="J1230" s="3"/>
-      <c r="K1230" s="3"/>
-      <c r="L1230" s="2"/>
-      <c r="M1230" s="2"/>
-      <c r="N1230" s="2"/>
-      <c r="O1230" s="2"/>
-    </row>
-    <row r="1231" spans="10:15" x14ac:dyDescent="0.25">
-      <c r="J1231" s="3"/>
-      <c r="K1231" s="3"/>
-      <c r="L1231" s="2"/>
-      <c r="M1231" s="2"/>
-      <c r="N1231" s="2"/>
-      <c r="O1231" s="2"/>
-    </row>
-    <row r="1232" spans="10:15" x14ac:dyDescent="0.25">
-      <c r="J1232" s="3"/>
-      <c r="K1232" s="3"/>
-      <c r="L1232" s="2"/>
-      <c r="M1232" s="2"/>
-      <c r="N1232" s="2"/>
-      <c r="O1232" s="2"/>
-    </row>
-    <row r="1233" spans="10:15" x14ac:dyDescent="0.25">
-      <c r="J1233" s="3"/>
-      <c r="K1233" s="3"/>
-      <c r="L1233" s="2"/>
-      <c r="M1233" s="2"/>
-      <c r="N1233" s="2"/>
-      <c r="O1233" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -13562,10 +13585,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:N333"/>
+  <dimension ref="A1:N340"/>
   <sheetViews>
-    <sheetView topLeftCell="A307" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A334" sqref="A334"/>
+    <sheetView topLeftCell="A301" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A336" sqref="A336:N340"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -25592,28 +25615,28 @@
         <v>0.3</v>
       </c>
       <c r="F330" s="4">
-        <v>-9.0899999999999998E-4</v>
+        <v>-9.0921413562799699E-4</v>
       </c>
       <c r="G330" s="4">
-        <v>3.3439800999999998E-2</v>
+        <v>3.3439800565223401E-2</v>
       </c>
       <c r="H330" s="6">
-        <v>0.99999633700000001</v>
+        <v>0.99999633700777302</v>
       </c>
       <c r="I330" s="3">
-        <v>90.966866019999998</v>
+        <v>192.8</v>
       </c>
       <c r="J330" s="3">
-        <v>14.907175779999999</v>
+        <v>22.05</v>
       </c>
       <c r="K330" s="2">
-        <v>7.3500000000000003E-8</v>
+        <v>7.3512048004431497E-8</v>
       </c>
       <c r="L330" s="2">
-        <v>6.6699999999999995E-8</v>
+        <v>6.6715037970513199E-8</v>
       </c>
       <c r="M330" s="2">
-        <v>6.7599999999999997E-8</v>
+        <v>6.7627642238887299E-8</v>
       </c>
       <c r="N330" t="s">
         <v>118</v>
@@ -25636,28 +25659,28 @@
         <v>0.3</v>
       </c>
       <c r="F331" s="4">
-        <v>4.0844599999999998E-3</v>
+        <v>4.0844602397185799E-3</v>
       </c>
       <c r="G331" s="4">
-        <v>3.4151391000000003E-2</v>
+        <v>3.4151391091771899E-2</v>
       </c>
       <c r="H331" s="6">
-        <v>0.999996577</v>
+        <v>0.99999657670818698</v>
       </c>
       <c r="I331" s="3">
-        <v>92.487341880000002</v>
+        <v>200.97</v>
       </c>
       <c r="J331" s="3">
-        <v>14.638382910000001</v>
+        <v>22.4499999999999</v>
       </c>
       <c r="K331" s="2">
-        <v>8.7499999999999996E-8</v>
+        <v>8.7515353186518001E-8</v>
       </c>
       <c r="L331" s="2">
-        <v>6.8400000000000004E-8</v>
+        <v>6.8449665999967694E-8</v>
       </c>
       <c r="M331" s="2">
-        <v>6.9100000000000003E-8</v>
+        <v>6.9123027790869602E-8</v>
       </c>
       <c r="N331" t="s">
         <v>118</v>
@@ -25680,28 +25703,28 @@
         <v>0.3</v>
       </c>
       <c r="F332" s="4">
-        <v>1.382994E-3</v>
+        <v>1.3829942295186101E-3</v>
       </c>
       <c r="G332" s="4">
-        <v>3.3964632000000002E-2</v>
+        <v>3.3964631553198101E-2</v>
       </c>
       <c r="H332" s="6">
-        <v>0.99999584799999996</v>
+        <v>0.99999584792267204</v>
       </c>
       <c r="I332" s="3">
-        <v>97.379619840000004</v>
+        <v>213.09</v>
       </c>
       <c r="J332" s="3">
-        <v>14.619490150000001</v>
+        <v>22.75</v>
       </c>
       <c r="K332" s="2">
-        <v>9.2000000000000003E-8</v>
+        <v>9.1962128578870695E-8</v>
       </c>
       <c r="L332" s="2">
-        <v>7.7200000000000003E-8</v>
+        <v>7.7225055450271696E-8</v>
       </c>
       <c r="M332" s="2">
-        <v>7.7099999999999996E-8</v>
+        <v>7.7141872727837706E-8</v>
       </c>
       <c r="N332" t="s">
         <v>118</v>
@@ -25724,30 +25747,255 @@
         <v>0.3</v>
       </c>
       <c r="F333" s="4">
-        <v>-1.3670819999999999E-3</v>
+        <v>-1.3670824311431001E-3</v>
       </c>
       <c r="G333" s="4">
-        <v>3.1934840999999999E-2</v>
+        <v>3.1934841181277998E-2</v>
       </c>
       <c r="H333" s="6">
-        <v>0.99999631899999997</v>
+        <v>0.99999631854180704</v>
       </c>
       <c r="I333" s="3">
-        <v>99.039443969999994</v>
+        <v>247.159999999999</v>
       </c>
       <c r="J333" s="3">
-        <v>14.70431685</v>
+        <v>21.5199999999999</v>
       </c>
       <c r="K333" s="2">
-        <v>7.6500000000000003E-8</v>
+        <v>7.6510758617587205E-8</v>
       </c>
       <c r="L333" s="2">
-        <v>7.1E-8</v>
+        <v>7.0950285523419098E-8</v>
       </c>
       <c r="M333" s="2">
-        <v>7.1600000000000006E-8</v>
+        <v>7.1614143243798606E-8</v>
       </c>
       <c r="N333" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="335" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A335" s="1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="336" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A336" t="s">
+        <v>0</v>
+      </c>
+      <c r="B336" t="s">
+        <v>1</v>
+      </c>
+      <c r="C336" t="s">
+        <v>11</v>
+      </c>
+      <c r="D336" t="s">
+        <v>2</v>
+      </c>
+      <c r="E336" t="s">
+        <v>3</v>
+      </c>
+      <c r="F336" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G336" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H336" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="I336" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="J336" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="K336" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="L336" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="M336" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="N336" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="337" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A337">
+        <v>2</v>
+      </c>
+      <c r="B337">
+        <v>1</v>
+      </c>
+      <c r="C337">
+        <v>1</v>
+      </c>
+      <c r="D337">
+        <v>710880</v>
+      </c>
+      <c r="E337">
+        <v>0.3</v>
+      </c>
+      <c r="F337" s="4">
+        <v>-9.0921413562799699E-4</v>
+      </c>
+      <c r="G337" s="4">
+        <v>3.3439800565223401E-2</v>
+      </c>
+      <c r="H337" s="6">
+        <v>0.99999633700777302</v>
+      </c>
+      <c r="I337" s="3">
+        <v>89.139999999999802</v>
+      </c>
+      <c r="J337" s="3">
+        <v>11.5700000000001</v>
+      </c>
+      <c r="K337" s="2">
+        <v>7.3512048004431497E-8</v>
+      </c>
+      <c r="L337" s="2">
+        <v>6.6715037970513199E-8</v>
+      </c>
+      <c r="M337" s="2">
+        <v>6.7627642238887299E-8</v>
+      </c>
+      <c r="N337" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="338" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A338">
+        <v>2</v>
+      </c>
+      <c r="B338">
+        <v>1</v>
+      </c>
+      <c r="C338">
+        <v>2</v>
+      </c>
+      <c r="D338">
+        <v>710880</v>
+      </c>
+      <c r="E338">
+        <v>0.3</v>
+      </c>
+      <c r="F338" s="4">
+        <v>4.0844602397185799E-3</v>
+      </c>
+      <c r="G338" s="4">
+        <v>3.4151391091771899E-2</v>
+      </c>
+      <c r="H338" s="6">
+        <v>0.99999657670818698</v>
+      </c>
+      <c r="I338" s="3">
+        <v>101.07</v>
+      </c>
+      <c r="J338" s="3">
+        <v>13.3200000000001</v>
+      </c>
+      <c r="K338" s="2">
+        <v>8.7515353186518001E-8</v>
+      </c>
+      <c r="L338" s="2">
+        <v>6.8449665999967694E-8</v>
+      </c>
+      <c r="M338" s="2">
+        <v>6.9123027790869602E-8</v>
+      </c>
+      <c r="N338" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="339" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A339">
+        <v>2</v>
+      </c>
+      <c r="B339">
+        <v>1</v>
+      </c>
+      <c r="C339">
+        <v>3</v>
+      </c>
+      <c r="D339">
+        <v>710880</v>
+      </c>
+      <c r="E339">
+        <v>0.3</v>
+      </c>
+      <c r="F339" s="4">
+        <v>1.3829942295186101E-3</v>
+      </c>
+      <c r="G339" s="4">
+        <v>3.3964631553198101E-2</v>
+      </c>
+      <c r="H339" s="6">
+        <v>0.99999584792267204</v>
+      </c>
+      <c r="I339" s="3">
+        <v>99.2800000000002</v>
+      </c>
+      <c r="J339" s="3">
+        <v>11.5199999999999</v>
+      </c>
+      <c r="K339" s="2">
+        <v>9.1962128578870695E-8</v>
+      </c>
+      <c r="L339" s="2">
+        <v>7.7225055450271696E-8</v>
+      </c>
+      <c r="M339" s="2">
+        <v>7.7141872727837706E-8</v>
+      </c>
+      <c r="N339" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="340" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A340">
+        <v>2</v>
+      </c>
+      <c r="B340">
+        <v>1</v>
+      </c>
+      <c r="C340">
+        <v>4</v>
+      </c>
+      <c r="D340">
+        <v>710880</v>
+      </c>
+      <c r="E340">
+        <v>0.3</v>
+      </c>
+      <c r="F340" s="4">
+        <v>-1.3670824311431001E-3</v>
+      </c>
+      <c r="G340" s="4">
+        <v>3.1934841181277998E-2</v>
+      </c>
+      <c r="H340" s="6">
+        <v>0.99999631854180704</v>
+      </c>
+      <c r="I340" s="3">
+        <v>112.44</v>
+      </c>
+      <c r="J340" s="3">
+        <v>10.809999999999899</v>
+      </c>
+      <c r="K340" s="2">
+        <v>7.6510758617587205E-8</v>
+      </c>
+      <c r="L340" s="2">
+        <v>7.0950285523419098E-8</v>
+      </c>
+      <c r="M340" s="2">
+        <v>7.1614143243798606E-8</v>
+      </c>
+      <c r="N340" t="s">
         <v>118</v>
       </c>
     </row>
@@ -25759,10 +26007,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{149088EA-EE89-4913-8BD8-AB9DFE4F2867}">
-  <dimension ref="A1:P44"/>
+  <dimension ref="A1:P53"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A14" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A43" sqref="A43:P44"/>
+      <selection activeCell="A52" sqref="A52:P53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -26743,7 +26991,7 @@
         <v>6.7599999999999997E-8</v>
       </c>
       <c r="G40" s="3">
-        <v>379.87327169999998</v>
+        <v>854.02</v>
       </c>
       <c r="H40" s="4">
         <v>-6.7400000000000001E-4</v>
@@ -26758,7 +27006,7 @@
         <v>7.0300000000000001E-8</v>
       </c>
       <c r="L40" s="5">
-        <v>1.1359060999999999</v>
+        <v>1.802</v>
       </c>
       <c r="M40" s="5">
         <v>0.22524235100000001</v>
@@ -26875,6 +27123,216 @@
         <v>0.249522060423856</v>
       </c>
       <c r="P44" s="5" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A47" s="1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>22</v>
+      </c>
+      <c r="B48" t="s">
+        <v>1</v>
+      </c>
+      <c r="C48" t="s">
+        <v>28</v>
+      </c>
+      <c r="D48" t="s">
+        <v>120</v>
+      </c>
+      <c r="E48" t="s">
+        <v>33</v>
+      </c>
+      <c r="F48" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G48" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="H48" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="I48" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="J48" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="K48" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="L48" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="M48" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="N48" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="O48" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="P48" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="49" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>2</v>
+      </c>
+      <c r="B49">
+        <v>1</v>
+      </c>
+      <c r="C49">
+        <v>4</v>
+      </c>
+      <c r="D49">
+        <v>10</v>
+      </c>
+      <c r="E49">
+        <v>60120</v>
+      </c>
+      <c r="F49" s="2">
+        <v>6.7627642238887299E-8</v>
+      </c>
+      <c r="G49" s="3">
+        <v>401.93</v>
+      </c>
+      <c r="H49" s="4">
+        <v>-6.73721630007402E-4</v>
+      </c>
+      <c r="I49" s="4">
+        <v>3.0206327936049601E-2</v>
+      </c>
+      <c r="J49" s="6">
+        <v>0.99999616928617796</v>
+      </c>
+      <c r="K49" s="2">
+        <v>7.0288925180441094E-8</v>
+      </c>
+      <c r="L49" s="5">
+        <v>0.85700000000001597</v>
+      </c>
+      <c r="M49" s="5">
+        <v>0.22524235144299601</v>
+      </c>
+      <c r="N49" s="5">
+        <v>0.47476441186685298</v>
+      </c>
+      <c r="O49" s="5">
+        <v>0.249522060423856</v>
+      </c>
+      <c r="P49" s="5" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="51" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A51" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="52" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>22</v>
+      </c>
+      <c r="B52" t="s">
+        <v>1</v>
+      </c>
+      <c r="C52" t="s">
+        <v>28</v>
+      </c>
+      <c r="D52" t="s">
+        <v>120</v>
+      </c>
+      <c r="E52" t="s">
+        <v>33</v>
+      </c>
+      <c r="F52" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G52" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="H52" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="I52" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="J52" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="K52" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="L52" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="M52" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="N52" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="O52" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="P52" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="53" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>2</v>
+      </c>
+      <c r="B53">
+        <v>1</v>
+      </c>
+      <c r="C53">
+        <v>4</v>
+      </c>
+      <c r="D53">
+        <v>10</v>
+      </c>
+      <c r="E53">
+        <v>60120</v>
+      </c>
+      <c r="F53" s="2">
+        <v>6.7627642238887299E-8</v>
+      </c>
+      <c r="G53" s="3">
+        <v>401.93</v>
+      </c>
+      <c r="H53" s="4">
+        <v>0.30653459518111098</v>
+      </c>
+      <c r="I53" s="4">
+        <v>0.98610453781241503</v>
+      </c>
+      <c r="J53" s="6">
+        <v>0.99743198707195901</v>
+      </c>
+      <c r="K53" s="2">
+        <v>3.8923043639431397E-5</v>
+      </c>
+      <c r="L53" s="5">
+        <v>0.83600000000010299</v>
+      </c>
+      <c r="M53" s="5">
+        <v>0.22524235144299601</v>
+      </c>
+      <c r="N53" s="5">
+        <v>0.47476441186685298</v>
+      </c>
+      <c r="O53" s="5">
+        <v>0.249522060423856</v>
+      </c>
+      <c r="P53" s="5" t="s">
         <v>118</v>
       </c>
     </row>
@@ -26885,10 +27343,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AAA7905-EEB3-4C3A-B027-599D0122CD07}">
-  <dimension ref="A1:Q63"/>
+  <dimension ref="A1:Q70"/>
   <sheetViews>
-    <sheetView topLeftCell="A23" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="N61" sqref="N61"/>
+    <sheetView topLeftCell="A41" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A67" sqref="A67:Q70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -28759,34 +29217,34 @@
         <v>10</v>
       </c>
       <c r="G54" s="2">
-        <v>6.7599999999999997E-8</v>
+        <v>6.7627642238887299E-8</v>
       </c>
       <c r="H54" s="6">
-        <v>379.87327169999998</v>
+        <v>854.02</v>
       </c>
       <c r="I54" s="4">
-        <v>-6.7400000000000001E-4</v>
+        <v>-6.73721630007402E-4</v>
       </c>
       <c r="J54" s="4">
-        <v>3.0206328000000001E-2</v>
+        <v>3.0206327936049601E-2</v>
       </c>
       <c r="K54" s="6">
-        <v>0.99999616899999999</v>
+        <v>0.99999616928617796</v>
       </c>
       <c r="L54" s="2">
-        <v>7.0300000000000001E-8</v>
+        <v>7.0288925180441094E-8</v>
       </c>
       <c r="M54" s="5">
-        <v>1.1359060999999999</v>
+        <v>1.8019999999999701</v>
       </c>
       <c r="N54" s="5">
-        <v>0.29125193399999999</v>
+        <v>0.29125193440910702</v>
       </c>
       <c r="O54" s="5">
-        <v>0.60563728900000002</v>
+        <v>0.60563728900474201</v>
       </c>
       <c r="P54" s="5">
-        <v>0.31438535499999998</v>
+        <v>0.31438535459563499</v>
       </c>
       <c r="Q54" t="s">
         <v>118</v>
@@ -28812,34 +29270,34 @@
         <v>10</v>
       </c>
       <c r="G55" s="2">
-        <v>6.7599999999999997E-8</v>
+        <v>6.7627642238887299E-8</v>
       </c>
       <c r="H55" s="6">
-        <v>379.87327169999998</v>
+        <v>854.02</v>
       </c>
       <c r="I55" s="4">
-        <v>-6.7400000000000001E-4</v>
+        <v>-6.73721630007402E-4</v>
       </c>
       <c r="J55" s="4">
-        <v>3.0206328000000001E-2</v>
+        <v>3.0206327936049601E-2</v>
       </c>
       <c r="K55" s="6">
-        <v>0.99999616899999999</v>
+        <v>0.99999616928617796</v>
       </c>
       <c r="L55" s="2">
-        <v>7.0300000000000001E-8</v>
+        <v>7.0288925180441094E-8</v>
       </c>
       <c r="M55" s="5">
-        <v>1.1359060999999999</v>
+        <v>1.8019999999999701</v>
       </c>
       <c r="N55" s="5">
-        <v>0.23886972000000001</v>
+        <v>0.23886971987010999</v>
       </c>
       <c r="O55" s="5">
-        <v>0.29259307600000001</v>
+        <v>0.29259307628201198</v>
       </c>
       <c r="P55" s="5">
-        <v>5.3723356E-2</v>
+        <v>5.3723356411901797E-2</v>
       </c>
       <c r="Q55" t="s">
         <v>118</v>
@@ -28865,34 +29323,34 @@
         <v>10</v>
       </c>
       <c r="G56" s="2">
-        <v>6.7599999999999997E-8</v>
+        <v>6.7627642238887299E-8</v>
       </c>
       <c r="H56" s="6">
-        <v>379.87327169999998</v>
+        <v>854.02</v>
       </c>
       <c r="I56" s="4">
-        <v>-6.7400000000000001E-4</v>
+        <v>-6.73721630007402E-4</v>
       </c>
       <c r="J56" s="4">
-        <v>3.0206328000000001E-2</v>
+        <v>3.0206327936049601E-2</v>
       </c>
       <c r="K56" s="6">
-        <v>0.99999616899999999</v>
+        <v>0.99999616928617796</v>
       </c>
       <c r="L56" s="2">
-        <v>7.0300000000000001E-8</v>
+        <v>7.0288925180441094E-8</v>
       </c>
       <c r="M56" s="5">
-        <v>1.1359060999999999</v>
+        <v>1.8019999999999701</v>
       </c>
       <c r="N56" s="5">
-        <v>0.1456054</v>
+        <v>0.14560540004977099</v>
       </c>
       <c r="O56" s="5">
-        <v>0.52606286999999996</v>
+        <v>0.52606287031380305</v>
       </c>
       <c r="P56" s="5">
-        <v>0.38045747000000002</v>
+        <v>0.38045747026403198</v>
       </c>
       <c r="Q56" t="s">
         <v>118</v>
@@ -29113,6 +29571,223 @@
       </c>
       <c r="Q63" t="s">
         <v>125</v>
+      </c>
+    </row>
+    <row r="66" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A66" s="1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="67" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>22</v>
+      </c>
+      <c r="B67" t="s">
+        <v>1</v>
+      </c>
+      <c r="C67" t="s">
+        <v>103</v>
+      </c>
+      <c r="D67" t="s">
+        <v>28</v>
+      </c>
+      <c r="E67" t="s">
+        <v>33</v>
+      </c>
+      <c r="F67" t="s">
+        <v>120</v>
+      </c>
+      <c r="G67" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H67" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="I67" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="J67" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="K67" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="L67" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="M67" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="N67" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="O67" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="P67" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q67" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="68" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <v>2</v>
+      </c>
+      <c r="B68">
+        <v>1</v>
+      </c>
+      <c r="C68" t="s">
+        <v>121</v>
+      </c>
+      <c r="D68">
+        <v>4</v>
+      </c>
+      <c r="E68">
+        <v>60120</v>
+      </c>
+      <c r="F68">
+        <v>10</v>
+      </c>
+      <c r="G68" s="2">
+        <v>6.7599999999999997E-8</v>
+      </c>
+      <c r="H68" s="6">
+        <v>401.93</v>
+      </c>
+      <c r="I68" s="4">
+        <v>-6.7400000000000001E-4</v>
+      </c>
+      <c r="J68" s="4">
+        <v>3.0206328000000001E-2</v>
+      </c>
+      <c r="K68" s="6">
+        <v>0.99999616899999999</v>
+      </c>
+      <c r="L68" s="2">
+        <v>7.0300000000000001E-8</v>
+      </c>
+      <c r="M68" s="5">
+        <v>0.85699999999999998</v>
+      </c>
+      <c r="N68" s="5">
+        <v>0.29125193399999999</v>
+      </c>
+      <c r="O68" s="5">
+        <v>0.60563728900000002</v>
+      </c>
+      <c r="P68" s="5">
+        <v>0.31438535499999998</v>
+      </c>
+      <c r="Q68" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="69" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A69">
+        <v>2</v>
+      </c>
+      <c r="B69">
+        <v>1</v>
+      </c>
+      <c r="C69" t="s">
+        <v>122</v>
+      </c>
+      <c r="D69">
+        <v>4</v>
+      </c>
+      <c r="E69">
+        <v>60120</v>
+      </c>
+      <c r="F69">
+        <v>10</v>
+      </c>
+      <c r="G69" s="2">
+        <v>6.7599999999999997E-8</v>
+      </c>
+      <c r="H69" s="6">
+        <v>401.93</v>
+      </c>
+      <c r="I69" s="4">
+        <v>-6.7400000000000001E-4</v>
+      </c>
+      <c r="J69" s="4">
+        <v>3.0206328000000001E-2</v>
+      </c>
+      <c r="K69" s="6">
+        <v>0.99999616899999999</v>
+      </c>
+      <c r="L69" s="2">
+        <v>7.0300000000000001E-8</v>
+      </c>
+      <c r="M69" s="5">
+        <v>0.85699999999999998</v>
+      </c>
+      <c r="N69" s="5">
+        <v>0.23886972000000001</v>
+      </c>
+      <c r="O69" s="5">
+        <v>0.29259307600000001</v>
+      </c>
+      <c r="P69" s="5">
+        <v>5.3723356E-2</v>
+      </c>
+      <c r="Q69" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="70" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A70">
+        <v>2</v>
+      </c>
+      <c r="B70">
+        <v>1</v>
+      </c>
+      <c r="C70" t="s">
+        <v>123</v>
+      </c>
+      <c r="D70">
+        <v>4</v>
+      </c>
+      <c r="E70">
+        <v>60120</v>
+      </c>
+      <c r="F70">
+        <v>10</v>
+      </c>
+      <c r="G70" s="2">
+        <v>6.7599999999999997E-8</v>
+      </c>
+      <c r="H70" s="6">
+        <v>401.93</v>
+      </c>
+      <c r="I70" s="4">
+        <v>-6.7400000000000001E-4</v>
+      </c>
+      <c r="J70" s="4">
+        <v>3.0206328000000001E-2</v>
+      </c>
+      <c r="K70" s="6">
+        <v>0.99999616899999999</v>
+      </c>
+      <c r="L70" s="2">
+        <v>7.0300000000000001E-8</v>
+      </c>
+      <c r="M70" s="5">
+        <v>0.85699999999999998</v>
+      </c>
+      <c r="N70" s="5">
+        <v>0.1456054</v>
+      </c>
+      <c r="O70" s="5">
+        <v>0.52606286999999996</v>
+      </c>
+      <c r="P70" s="5">
+        <v>0.38045747000000002</v>
+      </c>
+      <c r="Q70" t="s">
+        <v>118</v>
       </c>
     </row>
   </sheetData>

</xml_diff>